<commit_message>
bs env for sicmdp
</commit_message>
<xml_diff>
--- a/configs/bs_position.xlsx
+++ b/configs/bs_position.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12255"/>
+    <workbookView windowHeight="17655"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1183,7 +1183,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5" outlineLevelCol="2"/>
@@ -1201,57 +1201,57 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>25</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>5</v>
+        <v>200</v>
       </c>
       <c r="B3">
-        <v>4995</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>25</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>4995</v>
+        <v>0</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>200</v>
       </c>
       <c r="C4">
-        <v>25</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>4995</v>
+        <v>200</v>
       </c>
       <c r="B5">
-        <v>4995</v>
+        <v>200</v>
       </c>
       <c r="C5">
-        <v>25</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <v>2500</v>
+        <v>100</v>
       </c>
       <c r="B6">
-        <v>2500</v>
+        <v>100</v>
       </c>
       <c r="C6">
-        <v>25</v>
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>